<commit_message>
Creating the certificate for the giz students trained on robotics and ai
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MO_WIZZ\Documents\Python_Project\Certificate_creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD916246-C747-4C5C-9CF4-CD528A5F4A16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0491944F-C98B-4ED0-BF52-24B8365736AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="345" windowWidth="16320" windowHeight="12600" xr2:uid="{AD35F1AD-8936-4977-B81E-20400D95A481}"/>
+    <workbookView xWindow="3165" yWindow="9345" windowWidth="24015" windowHeight="12600" xr2:uid="{AD35F1AD-8936-4977-B81E-20400D95A481}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>EMAIL</t>
   </si>
@@ -72,13 +72,31 @@
     <t>ikotaestate@gmail.com</t>
   </si>
   <si>
-    <t>Edutech  Christain</t>
-  </si>
-  <si>
     <t>Onyekachi  Ekenechukwu</t>
   </si>
   <si>
-    <t>Chinedu  Patrick</t>
+    <t>CERTNO</t>
+  </si>
+  <si>
+    <t>Chinonyelum Ejimuda</t>
+  </si>
+  <si>
+    <t>Chinedu  Michael</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>20th August, 2020</t>
+  </si>
+  <si>
+    <t>https://roboticscentre.org/       (20082021,009)</t>
+  </si>
+  <si>
+    <t>https://roboticscentre.org/    (20082021,008)</t>
+  </si>
+  <si>
+    <t>https://roboticscentre.org/    (20082021,010)</t>
   </si>
 </sst>
 </file>
@@ -441,26 +459,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0550A8C-DE34-4EF4-AD7E-27F9BA310555}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="38.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -491,10 +511,16 @@
       <c r="J1" t="s">
         <v>11</v>
       </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -523,10 +549,16 @@
       <c r="J2" t="s">
         <v>12</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -555,10 +587,13 @@
       <c r="J3" t="s">
         <v>13</v>
       </c>
+      <c r="K3" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -586,6 +621,9 @@
       </c>
       <c r="J4" t="s">
         <v>13</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -593,6 +631,9 @@
     <hyperlink ref="B3" r:id="rId1" xr:uid="{3A362B3A-2CCA-4182-9D0D-965EB8AA9836}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{4E436413-9BE6-40BF-BE95-2D5C263773BC}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{AEC58459-40A5-4176-9F3F-693C5FC77747}"/>
+    <hyperlink ref="K2" r:id="rId4" xr:uid="{0515AA85-2377-40B1-B03B-9132D5C111EC}"/>
+    <hyperlink ref="K3" r:id="rId5" xr:uid="{B23B8946-D0C8-4EF7-9310-D97BBD405AB8}"/>
+    <hyperlink ref="K4" r:id="rId6" xr:uid="{38F15201-0A96-4241-B0F0-0CF097A82FE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>